<commit_message>
automation of dashboard page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,21 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>password</t>
+    <t>(+91)India</t>
   </si>
   <si>
-    <t>phone</t>
+    <t>3239131871</t>
   </si>
   <si>
-    <t>pass@123</t>
+    <t>Pass@123</t>
   </si>
   <si>
-    <t>Country code</t>
+    <t>8457528454</t>
   </si>
   <si>
-    <t>(+91)India</t>
+    <t>(+1) United  States</t>
   </si>
 </sst>
 </file>
@@ -371,32 +371,32 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I11" activeCellId="1" sqref="C9 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>3239131871</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -404,8 +404,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added pom and DD concepta for automation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Khushboo\vc_doctor_automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vc_doctor_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>(+91)India</t>
-  </si>
-  <si>
     <t>3239131871</t>
   </si>
   <si>
@@ -39,6 +36,9 @@
   </si>
   <si>
     <t>(+1) United  States</t>
+  </si>
+  <si>
+    <t>(+1)India</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" activeCellId="1" sqref="C9 I11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,24 +382,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>